<commit_message>
Fixed mysterious blank plus z BOM. Also added date and notes fields to minus z BOM.
</commit_message>
<xml_diff>
--- a/oresat0-minusz-end-cap-bom.xlsx
+++ b/oresat0-minusz-end-cap-bom.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monke\Documents\Oresat_Git\oresat-endcaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CA2D44-6495-4AAF-9A65-98BFED660898}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B25936-FBBC-464C-ACC7-3BBE4A2E0EB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$7:$I$17</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$7:$I$17</definedName>
   </definedNames>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
   <si>
     <t>Description</t>
   </si>
@@ -232,6 +231,15 @@
   </si>
   <si>
     <t>952-3875-1-ND</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>First version of BOM</t>
   </si>
 </sst>
 </file>
@@ -282,20 +290,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <b/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -319,7 +326,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -361,18 +370,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F97684FC-5F6A-45BB-B9CF-1F2A70239A34}" name="oresat0_minusz_end_cap" displayName="oresat0_minusz_end_cap" ref="A7:I17" tableType="queryTable" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F97684FC-5F6A-45BB-B9CF-1F2A70239A34}" name="oresat0_minusz_end_cap" displayName="oresat0_minusz_end_cap" ref="A7:I17" tableType="queryTable" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A7:I17" xr:uid="{60799C6D-FCC5-41B3-A3F9-78F1453222FD}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{EC5CB959-8F03-45C3-92F6-8B7E21E36BCB}" uniqueName="1" name="Cnt" queryTableFieldId="1"/>
-    <tableColumn id="5" xr3:uid="{4AD4F4CF-F11F-4C59-A0A4-29E780CD245C}" uniqueName="5" name="Part References" queryTableFieldId="5" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{DEF7B512-226F-47BD-A513-4D8A8C4BAA94}" uniqueName="14" name="P/DNP" queryTableFieldId="15" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{7950441B-3519-4FE1-9114-877EB8E7975F}" uniqueName="9" name="Mfg" queryTableFieldId="9" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{85D04B1D-8B0A-4D1F-8D91-6F1144AC9ABA}" uniqueName="10" name="Mfg PN" queryTableFieldId="10" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{1ED24844-B1A2-485E-A337-94BE25CD80A6}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{7921D25D-A454-4EAA-AB49-EE2EDE882F94}" uniqueName="15" name="Generic" queryTableFieldId="17" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{14565EFB-23DB-44EB-94A1-39B7BEF08052}" uniqueName="7" name="DIS" queryTableFieldId="7" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{5939C906-0F2C-4A86-A4BA-0C3D9F50FEED}" uniqueName="8" name="DPN" queryTableFieldId="8" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{4AD4F4CF-F11F-4C59-A0A4-29E780CD245C}" uniqueName="5" name="Part References" queryTableFieldId="5" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{DEF7B512-226F-47BD-A513-4D8A8C4BAA94}" uniqueName="14" name="P/DNP" queryTableFieldId="15" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{7950441B-3519-4FE1-9114-877EB8E7975F}" uniqueName="9" name="Mfg" queryTableFieldId="9" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{85D04B1D-8B0A-4D1F-8D91-6F1144AC9ABA}" uniqueName="10" name="Mfg PN" queryTableFieldId="10" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{1ED24844-B1A2-485E-A337-94BE25CD80A6}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{7921D25D-A454-4EAA-AB49-EE2EDE882F94}" uniqueName="15" name="Generic" queryTableFieldId="17" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{14565EFB-23DB-44EB-94A1-39B7BEF08052}" uniqueName="7" name="DIS" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{5939C906-0F2C-4A86-A4BA-0C3D9F50FEED}" uniqueName="8" name="DPN" queryTableFieldId="8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -643,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71830409-EC83-4E17-B2C8-D94ABB34AD5E}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -995,6 +1004,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="19" spans="1:9">
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>23</v>
@@ -1003,6 +1020,12 @@
     <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>24</v>
+      </c>
+      <c r="B21" s="4">
+        <v>44071</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1011,18 +1034,6 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>